<commit_message>
add new page so that Jim can compare raw html (or other text)
</commit_message>
<xml_diff>
--- a/Tests/book.xlsx
+++ b/Tests/book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\spreadsheet-comparison-tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{714C9367-143B-4C19-889B-B6F3776155B6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C394856A-A9C2-4154-93FB-FEB4AABA4ADC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CCA589C1-A5BD-403E-B054-6E1BD644C00F}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
         <v>51</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" ref="B5:D12" si="0">ROW()&amp;COLUMN()</f>
+        <f t="shared" ref="B5:D9" si="0">ROW()&amp;COLUMN()</f>
         <v>52</v>
       </c>
       <c r="C5" t="str">
@@ -462,7 +462,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f t="shared" ref="A6:A12" si="1">ROW()&amp;COLUMN()</f>
+        <f t="shared" ref="A6:A9" si="1">ROW()&amp;COLUMN()</f>
         <v>61</v>
       </c>
       <c r="B6" t="str">

</xml_diff>